<commit_message>
Added basic output board
</commit_message>
<xml_diff>
--- a/lichtenstein_onion-bom.xlsx
+++ b/lichtenstein_onion-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Electronics/EAGLE/lichtenstein_onion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D25052EC-AA5B-A543-8E3B-DD4A3A3F10F6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4E67B919-24F7-7B43-96AE-9DCBB81BD9E2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28360"/>
   </bookViews>
@@ -1233,7 +1233,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Fixed bulk capacitor footprints; made +V for output channels independent on output board
</commit_message>
<xml_diff>
--- a/lichtenstein_onion-bom.xlsx
+++ b/lichtenstein_onion-bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/lichtenstein/lichtenstein-omega2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBB9A7A7-380B-074A-B56F-8DCDCAC66C79}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F365A1E-43C6-3649-9F30-F13D7E0B2DE4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lichtenstein_onion" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="116">
-  <si>
-    <t>Partlist exported from /Users/tristan/EAGLE/lichtenstein-omega2/lichtenstein_onion.sch at 20180526 1156</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="120">
   <si>
     <t>Part</t>
   </si>
@@ -368,12 +365,27 @@
   </si>
   <si>
     <t>353-OM-O2P</t>
+  </si>
+  <si>
+    <t>47µF</t>
+  </si>
+  <si>
+    <t>CPOL-EUCT7343</t>
+  </si>
+  <si>
+    <t>CT7343</t>
+  </si>
+  <si>
+    <t>581-TAJD476M016RNJV</t>
+  </si>
+  <si>
+    <t>Partlist exported from /Users/tristan/EAGLE/lichtenstein-omega2/lichtenstein_onion.sch at 20180529 2252</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="12"/>
@@ -883,9 +895,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -899,6 +908,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1253,19 +1265,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
     <col min="5" max="5" width="59" customWidth="1"/>
     <col min="6" max="6" width="29.83203125" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -1273,1050 +1285,1060 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="F12" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="5" t="s">
+      <c r="F16" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1"/>
+      <c r="F18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
+      <c r="H19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="8"/>
+      <c r="F23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="5" t="s">
-        <v>62</v>
+      <c r="A24" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="8"/>
+      <c r="F24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="5" t="s">
-        <v>63</v>
+      <c r="A25" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="8"/>
+      <c r="F25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="5" t="s">
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F28" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="5" t="s">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F29" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="5" t="s">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="5" t="s">
+      <c r="F30" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="F35" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="8"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="F36" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="8"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="F37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="F41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="8"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="F42" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="8"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="8"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="8"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="8"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="8"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="8"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="8"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="5" t="s">
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="8"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="5" t="s">
+      <c r="B43" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="8"/>
-    </row>
-    <row r="44" spans="1:9" ht="32">
-      <c r="A44" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="8"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="8"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F46" s="7" t="s">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="8"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F47" s="7" t="s">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="7"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="8"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="5" t="s">
+      <c r="B48" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F48" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="8"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaned up output board; added pull-ups to inputs on Lichtenstein board; moved some decoupling caps on FPGA output board
</commit_message>
<xml_diff>
--- a/lichtenstein_onion-bom.xlsx
+++ b/lichtenstein_onion-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/lichtenstein/lichtenstein-omega2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F365A1E-43C6-3649-9F30-F13D7E0B2DE4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB0C657-853C-0A4D-84DC-9D13915D426E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="129">
   <si>
     <t>Part</t>
   </si>
@@ -226,9 +226,6 @@
     <t>RESISTOR, European symbol</t>
   </si>
   <si>
-    <t>652-CR0805FX-1002ELF</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -283,18 +280,6 @@
     <t>R13</t>
   </si>
   <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -379,14 +364,56 @@
     <t>581-TAJD476M016RNJV</t>
   </si>
   <si>
-    <t>Partlist exported from /Users/tristan/EAGLE/lichtenstein-omega2/lichtenstein_onion.sch at 20180529 2252</t>
+    <t>RN1</t>
+  </si>
+  <si>
+    <t>RN2</t>
+  </si>
+  <si>
+    <t>Chip Resistor Array 4 Single Resistor</t>
+  </si>
+  <si>
+    <t>Partlist exported from /Users/tristan/EAGLE/lichtenstein-omega2/lichtenstein_onion.sch at 20180530 2108</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>MOUNT-HOLE2.8</t>
+  </si>
+  <si>
+    <t>2,8</t>
+  </si>
+  <si>
+    <t>MOUNTING HOLE with drill center marker</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>CTS742C083</t>
+  </si>
+  <si>
+    <t>71-CRA04S0803103GRT7</t>
+  </si>
+  <si>
+    <t>RN3</t>
+  </si>
+  <si>
+    <t>SWCH-08441</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -517,14 +544,6 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -887,30 +906,46 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1266,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1279,22 +1314,22 @@
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" customWidth="1"/>
     <col min="5" max="5" width="59" customWidth="1"/>
-    <col min="6" max="6" width="29.83203125" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" style="10" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="A1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
@@ -1312,7 +1347,7 @@
       <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1338,7 +1373,7 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="6"/>
@@ -1361,7 +1396,7 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="6"/>
@@ -1373,19 +1408,19 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>118</v>
+      <c r="F6" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1407,7 +1442,7 @@
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="6"/>
@@ -1419,19 +1454,19 @@
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>118</v>
+      <c r="F8" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1445,15 +1480,15 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="6"/>
@@ -1476,7 +1511,7 @@
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="6"/>
@@ -1499,7 +1534,7 @@
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="6"/>
@@ -1511,7 +1546,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -1522,8 +1557,8 @@
       <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>118</v>
+      <c r="F12" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1545,7 +1580,7 @@
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="6"/>
@@ -1568,7 +1603,7 @@
       <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="6"/>
@@ -1591,7 +1626,7 @@
       <c r="E15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="6"/>
@@ -1603,19 +1638,19 @@
         <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>118</v>
+      <c r="F16" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1623,110 +1658,106 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>38</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F17" s="9"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="6" t="s">
-        <v>42</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>47</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>52</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>57</v>
+        <v>37</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -1734,20 +1765,18 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>59</v>
+        <v>41</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1755,41 +1784,47 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -1797,7 +1832,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
@@ -1809,8 +1844,8 @@
       <c r="E25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>59</v>
+      <c r="F25" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -1818,22 +1853,20 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -1841,22 +1874,20 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -1864,22 +1895,20 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -1887,22 +1916,20 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -1910,10 +1937,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>65</v>
@@ -1924,8 +1951,8 @@
       <c r="E30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>74</v>
+      <c r="F30" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -1933,10 +1960,10 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>65</v>
@@ -1947,8 +1974,8 @@
       <c r="E31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>77</v>
+      <c r="F31" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1956,10 +1983,10 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>65</v>
@@ -1970,8 +1997,8 @@
       <c r="E32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>77</v>
+      <c r="F32" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -1979,10 +2006,10 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>65</v>
@@ -1993,8 +2020,8 @@
       <c r="E33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>77</v>
+      <c r="F33" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -2002,10 +2029,10 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>65</v>
@@ -2016,8 +2043,8 @@
       <c r="E34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>74</v>
+      <c r="F34" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -2025,10 +2052,10 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>65</v>
@@ -2039,8 +2066,8 @@
       <c r="E35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>83</v>
+      <c r="F35" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -2048,10 +2075,10 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>65</v>
@@ -2062,8 +2089,8 @@
       <c r="E36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>83</v>
+      <c r="F36" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
@@ -2071,10 +2098,10 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>65</v>
@@ -2085,8 +2112,8 @@
       <c r="E37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>83</v>
+      <c r="F37" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -2094,10 +2121,10 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>65</v>
@@ -2108,8 +2135,8 @@
       <c r="E38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>83</v>
+      <c r="F38" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -2117,10 +2144,10 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>65</v>
@@ -2131,8 +2158,8 @@
       <c r="E39" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>83</v>
+      <c r="F39" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -2140,10 +2167,10 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>65</v>
@@ -2154,8 +2181,8 @@
       <c r="E40" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>74</v>
+      <c r="F40" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -2163,10 +2190,10 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>65</v>
@@ -2177,8 +2204,8 @@
       <c r="E41" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>83</v>
+      <c r="F41" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -2186,10 +2213,10 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>65</v>
@@ -2200,8 +2227,8 @@
       <c r="E42" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>83</v>
+      <c r="F42" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -2209,22 +2236,22 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="4" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>95</v>
+        <v>116</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -2232,20 +2259,22 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C44" s="1" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>100</v>
+        <v>116</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -2253,39 +2282,45 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C45" s="1" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F45" s="6"/>
+        <v>116</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="C46" s="1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>106</v>
+        <v>89</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -2293,47 +2328,101 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="4" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="G47" s="6"/>
+        <v>94</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="H47" s="6"/>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>114</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="F48" s="9"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="14"/>
+      <c r="C50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Got rid of resistor networks on lichtenstein board
</commit_message>
<xml_diff>
--- a/lichtenstein_onion-bom.xlsx
+++ b/lichtenstein_onion-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/lichtenstein/lichtenstein-omega2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB0C657-853C-0A4D-84DC-9D13915D426E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA259E81-B6B7-7944-B99F-918FB1A0B386}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lichtenstein_onion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="137">
   <si>
     <t>Part</t>
   </si>
@@ -364,15 +364,6 @@
     <t>581-TAJD476M016RNJV</t>
   </si>
   <si>
-    <t>RN1</t>
-  </si>
-  <si>
-    <t>RN2</t>
-  </si>
-  <si>
-    <t>Chip Resistor Array 4 Single Resistor</t>
-  </si>
-  <si>
     <t>Partlist exported from /Users/tristan/EAGLE/lichtenstein-omega2/lichtenstein_onion.sch at 20180530 2108</t>
   </si>
   <si>
@@ -397,16 +388,49 @@
     <t>H4</t>
   </si>
   <si>
-    <t>CTS742C083</t>
-  </si>
-  <si>
-    <t>71-CRA04S0803103GRT7</t>
-  </si>
-  <si>
-    <t>RN3</t>
-  </si>
-  <si>
     <t>SWCH-08441</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-1002ELF</t>
+  </si>
+  <si>
+    <t>MCP23017</t>
   </si>
 </sst>
 </file>
@@ -936,9 +960,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -946,6 +967,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1301,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F51"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1320,16 +1344,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="A1" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
@@ -1658,19 +1682,19 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="6"/>
@@ -1679,19 +1703,19 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="6"/>
@@ -1700,19 +1724,19 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="6"/>
@@ -1721,19 +1745,19 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="6"/>
@@ -1767,7 +1791,9 @@
       <c r="A22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
@@ -2236,22 +2262,22 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="4" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -2259,22 +2285,22 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="4" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
@@ -2282,22 +2308,22 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -2305,22 +2331,22 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="4" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -2328,99 +2354,306 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C47" s="1" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>128</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C48" s="1" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F48" s="9"/>
+        <v>67</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="13" t="s">
+    <row r="49" spans="1:9">
+      <c r="A49" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="7"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H56" s="6"/>
+      <c r="I56" s="7"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" s="9"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="7"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="1" t="s">
+      <c r="B58" s="13"/>
+      <c r="C58" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F58" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="13" t="s">
+    <row r="59" spans="1:9">
+      <c r="A59" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="1" t="s">
+      <c r="B59" s="13"/>
+      <c r="C59" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F59" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="13" t="s">
+    <row r="60" spans="1:9">
+      <c r="A60" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B60" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C60" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D60" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E60" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F60" s="11" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>